<commit_message>
cleaning up data, strarting vis
</commit_message>
<xml_diff>
--- a/random-subset.xlsx
+++ b/random-subset.xlsx
@@ -8,19 +8,57 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/dev/TEDvis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDA4B53-EAD5-6848-8E3A-177AF17D3C5B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D597321A-1872-214A-8481-81CB747F38C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+  <si>
+    <t>Why do people succeed? Is it because they're smart? Or are they just lucky? Neither. Analyst Richard St. John condenses years of interviews into an unmissable 3-minute slideshow on the real secrets of success.</t>
+  </si>
+  <si>
+    <t>TED2005</t>
+  </si>
+  <si>
+    <t>Richard St. John</t>
+  </si>
+  <si>
+    <t>Richard St. John: 8 secrets of success</t>
+  </si>
+  <si>
+    <t>[{'id': 7, 'name': 'Funny', 'count': 2966}, {'id': 1, 'name': 'Beautiful', 'count': 576}, {'id': 21, 'name': 'Unconvincing', 'count': 213}, {'id': 8, 'name': 'Informative', 'count': 1912}, {'id': 10, 'name': 'Inspiring', 'count': 4978}, {'id': 2, 'name': 'Confusing', 'count': 43}, {'id': 22, 'name': 'Fascinating', 'count': 777}, {'id': 9, 'name': 'Ingenious', 'count': 638}, {'id': 3, 'name': 'Courageous', 'count': 457}, {'id': 11, 'name': 'Longwinded', 'count': 27}, {'id': 24, 'name': 'Persuasive', 'count': 1433}, {'id': 23, 'name': 'Jaw-dropping', 'count': 251}, {'id': 25, 'name': 'OK', 'count': 685}, {'id': 26, 'name': 'Obnoxious', 'count': 57}]</t>
+  </si>
+  <si>
+    <t>[{'id': 66, 'hero': 'https://pe.tedcdn.com/images/ted/6b6eb940bceab359ca676a9b486aae475c1df883_2880x1620.jpg', 'speaker': 'Ken Robinson', 'title': 'Do schools kill creativity?', 'duration': 1164, 'slug': 'ken_robinson_says_schools_kill_creativity', 'viewed_count': 47227171}, {'id': 202, 'hero': 'https://pe.tedcdn.com/images/ted/87205c20e5b3e1b63d04da23c04b22956087f0be_2880x1620.jpg', 'speaker': 'Gever Tulley', 'title': '5 dangerous things you should let your kids do', 'duration': 558, 'slug': 'gever_tulley_on_5_dangerous_things_for_kids', 'viewed_count': 4364853}, {'id': 93, 'hero': 'https://pe.tedcdn.com/images/ted/bf2541157cdf5741f11ddea013c19b4ce5201be4_2880x1620.jpg', 'speaker': 'Barry Schwartz', 'title': 'The paradox of choice', 'duration': 1177, 'slug': 'barry_schwartz_on_the_paradox_of_choice', 'viewed_count': 10000711}, {'id': 572, 'hero': 'https://pe.tedcdn.com/images/ted/6c5a57b8edbb8082ef49b64994c3a1957f5e13a9_1600x1200.jpg', 'speaker': 'Richard St. John', 'title': 'Success is a continuous journey', 'duration': 237, 'slug': 'richard_st_john_success_is_a_continuous_journey', 'viewed_count': 3661589}, {'id': 2638, 'hero': 'https://pe.tedcdn.com/images/ted/f3b1cafe89d952edc479031dbd2df69faf730d74_2880x1620.jpg', 'speaker': 'Jia Jiang', 'title': 'What I learned from 100 days of rejection', 'duration': 931, 'slug': 'jia_jiang_what_i_learned_from_100_days_of_rejection', 'viewed_count': 3464229}, {'id': 2182, 'hero': 'https://pe.tedcdn.com/images/ted/07ece83dd77f758dd2c92e3fcb0ee6b404dc49a2_2880x1620.jpg', 'speaker': 'Ricardo Semler', 'title': 'How to run a company with (almost) no rules', 'duration': 1302, 'slug': 'ricardo_semler_how_to_run_a_company_with_almost_no_rules', 'viewed_count': 2610205}]</t>
+  </si>
+  <si>
+    <t>Marketer, success analyst</t>
+  </si>
+  <si>
+    <t>['business', 'culture', 'entertainment', 'happiness', 'psychology', 'success', 'work']</t>
+  </si>
+  <si>
+    <t>8 secrets of success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ted.com/talks/richard_st_john_s_8_secrets_of_success
+</t>
+  </si>
   <si>
     <t>How do you deal with a bully without becoming a thug? In this wise and soulful talk, peace activist Scilla Elworthy maps out the skills we need -- as nations and individuals -- to fight extreme force without using force in return. To answer the question of why and how nonviolence works, she evokes historical heroes -- Aung San Suu Kyi, Mahatma Gandhi, Nelson Mandela -- and the personal philosophies that powered their peaceful protests.</t>
   </si>
@@ -288,13 +326,25 @@
   </si>
   <si>
     <t>views</t>
+  </si>
+  <si>
+    <t>film_date_unix</t>
+  </si>
+  <si>
+    <t>duration_min</t>
+  </si>
+  <si>
+    <t>views_per_min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="yyyy/mm/dd;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -314,6 +364,11 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -337,11 +392,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,453 +716,618 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="16" max="16" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="16" max="16" width="102.1640625" customWidth="1"/>
+    <col min="18" max="18" width="84.1640625" customWidth="1"/>
+    <col min="20" max="20" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10841210</v>
+      </c>
+      <c r="C2" s="1">
+        <v>578</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>210</v>
+      </c>
+      <c r="F2" s="1">
+        <f>B2/E2</f>
+        <v>51624.809523809527</v>
+      </c>
+      <c r="G2" s="1">
+        <f>E2/60</f>
+        <v>3.5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <f>(J2/86400)+DATE(1970,1,1)</f>
+        <v>38406</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1109116800</v>
+      </c>
+      <c r="K2" s="1">
+        <v>66</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1166055060</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3769987</v>
+      </c>
+      <c r="C3" s="1">
+        <v>919</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1">
+        <v>992</v>
+      </c>
+      <c r="F3" s="1">
+        <f>B3/E3</f>
+        <v>3800.390120967742</v>
+      </c>
+      <c r="G3" s="1">
+        <f>E3/60</f>
+        <v>16.533333333333335</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I9" si="0">(J3/86400)+DATE(1970,1,1)</f>
+        <v>38772</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1140739200</v>
+      </c>
+      <c r="K3" s="1">
+        <v>31</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1152490260</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1145261</v>
+      </c>
+      <c r="C4" s="1">
+        <v>203</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>947</v>
+      </c>
+      <c r="F4" s="1">
+        <f>B4/E4</f>
+        <v>1209.3569165786694</v>
+      </c>
+      <c r="G4" s="1">
+        <f>E4/60</f>
+        <v>15.783333333333333</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="0"/>
+        <v>41019</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1334880000</v>
+      </c>
+      <c r="K4" s="1">
+        <v>32</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1344179026</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1049847</v>
+      </c>
+      <c r="C5" s="1">
+        <v>538</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1102</v>
+      </c>
+      <c r="F5" s="1">
+        <f>B5/E5</f>
+        <v>952.67422867513608</v>
+      </c>
+      <c r="G5" s="1">
+        <f>E5/60</f>
+        <v>18.366666666666667</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="0"/>
+        <v>40374</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1279152000</v>
+      </c>
+      <c r="K5" s="1">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1282038540</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1">
+        <v>642744</v>
+      </c>
+      <c r="C6" s="1">
+        <v>84</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1115</v>
+      </c>
+      <c r="F6" s="1">
+        <f>B6/E6</f>
+        <v>576.45201793721969</v>
+      </c>
+      <c r="G6" s="1">
+        <f>E6/60</f>
+        <v>18.583333333333332</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="0"/>
+        <v>40276</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1270684800</v>
+      </c>
+      <c r="K6" s="1">
+        <v>26</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1272442140</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="1">
+        <v>642201</v>
+      </c>
+      <c r="C7" s="1">
+        <v>94</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E7" s="1">
+        <v>1318</v>
+      </c>
+      <c r="F7" s="1">
+        <f>B7/E7</f>
+        <v>487.25417298937782</v>
+      </c>
+      <c r="G7" s="1">
+        <f>E7/60</f>
+        <v>21.966666666666665</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>38019</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1075680000</v>
+      </c>
+      <c r="K7" s="1">
+        <v>20</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="M7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="N7" s="1">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1229907600</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="Q7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="R7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="S7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="T7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>86</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
-        <v>203</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="1">
+        <v>404402</v>
+      </c>
+      <c r="C8" s="1">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1477</v>
+      </c>
+      <c r="F8" s="1">
+        <f>B8/E8</f>
+        <v>273.79959377115773</v>
+      </c>
+      <c r="G8" s="1">
+        <f>E8/60</f>
+        <v>24.616666666666667</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>37289</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1012608000</v>
+      </c>
+      <c r="K8" s="1">
+        <v>18</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1181625060</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="1">
+        <v>148971</v>
+      </c>
+      <c r="C9" s="1">
+        <v>46</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1013</v>
+      </c>
+      <c r="F9" s="1">
+        <f>B9/E9</f>
+        <v>147.05923000987167</v>
+      </c>
+      <c r="G9" s="1">
+        <f>E9/60</f>
+        <v>16.883333333333333</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>40635</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1301702400</v>
+      </c>
+      <c r="K9" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
-        <v>947</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="L9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N9" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
-        <v>1334880000</v>
-      </c>
-      <c r="F2" s="1">
-        <v>32</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1344179026</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>1145261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
-        <v>84</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1115</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1270684800</v>
-      </c>
-      <c r="F3" s="1">
-        <v>26</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1272442140</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>642744</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
-        <v>919</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1">
-        <v>992</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1140739200</v>
-      </c>
-      <c r="F4" s="1">
-        <v>31</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1">
-        <v>1152490260</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>3769987</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="1">
-        <v>538</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1102</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1279152000</v>
-      </c>
-      <c r="F5" s="1">
-        <v>30</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1">
-        <v>1282038540</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>1049847</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1477</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1012608000</v>
-      </c>
-      <c r="F6" s="1">
-        <v>18</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1">
-        <v>1181625060</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>404402</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
-        <v>46</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1013</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1301702400</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="O9" s="1">
         <v>1320501469</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>148971</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
-        <v>94</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1318</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1075680000</v>
-      </c>
-      <c r="F8" s="1">
-        <v>20</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1229907600</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M8" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="T9" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>642201</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="B2:T14">
+    <sortCondition descending="1" ref="F2:F14"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="P3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="P4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="P5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="P6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="P7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="P8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="T4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="T6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="T3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="T5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="T8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="T9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="T7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="T2" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>